<commit_message>
25.02.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/February/All Details/25.02.2020/MC Balance Transfer Feb'2020.xlsx
+++ b/2020/February/All Details/25.02.2020/MC Balance Transfer Feb'2020.xlsx
@@ -1193,7 +1193,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1205,7 +1205,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1228,14 +1228,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1543,9 +1543,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G52" sqref="G51:H52"/>
+      <selection pane="bottomLeft" activeCell="G102" sqref="G101:G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3510,17 +3510,17 @@
         <v>104</v>
       </c>
       <c r="B26" s="2">
-        <v>219745</v>
+        <v>259395</v>
       </c>
       <c r="C26" s="2">
-        <v>273225</v>
+        <v>317225</v>
       </c>
       <c r="D26" s="2">
         <v>640</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>273865</v>
+        <v>317865</v>
       </c>
       <c r="F26" s="127"/>
       <c r="G26" s="19"/>
@@ -3997,11 +3997,11 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>8332120</v>
+        <v>8371770</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>8241998</v>
+        <v>8285998</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
@@ -4009,11 +4009,11 @@
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>8267923</v>
+        <v>8311923</v>
       </c>
       <c r="F33" s="94">
         <f>B33-E33</f>
-        <v>64197</v>
+        <v>59847</v>
       </c>
       <c r="G33" s="114"/>
       <c r="H33" s="124"/>
@@ -4778,7 +4778,7 @@
       <c r="A44" s="73"/>
       <c r="B44" s="74"/>
       <c r="C44" s="75">
-        <v>2646</v>
+        <v>5296</v>
       </c>
       <c r="D44" s="76"/>
       <c r="E44" s="3"/>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="B60" s="43"/>
       <c r="C60" s="98">
-        <v>190000</v>
+        <v>183000</v>
       </c>
       <c r="D60" s="99" t="s">
         <v>104</v>
@@ -8635,7 +8635,7 @@
       <c r="B98" s="154"/>
       <c r="C98" s="45">
         <f>SUM(C37:C97)</f>
-        <v>1966170</v>
+        <v>1961820</v>
       </c>
       <c r="D98" s="41"/>
       <c r="F98" s="23"/>
@@ -8770,7 +8770,7 @@
       <c r="B100" s="152"/>
       <c r="C100" s="42">
         <f>C98+L121</f>
-        <v>1966170</v>
+        <v>1961820</v>
       </c>
       <c r="D100" s="26"/>
       <c r="F100" s="24"/>

</xml_diff>